<commit_message>
Separated Test Cases by Environment
</commit_message>
<xml_diff>
--- a/Data Files/RADI8代理编号对照表.xlsx
+++ b/Data Files/RADI8代理编号对照表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack.c/git/Katalon_API_Testing/Data Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA9E8AF-78D7-144A-9D5B-65A3B93B0A88}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EBF679-1AC5-CC4C-A8AF-D287AB73D367}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,35 +80,35 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="vicwu - 個人檢視畫面" guid="{8817F74E-6F61-4E32-8724-D0D706F320DB}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Jake - 個人檢視畫面" guid="{1DF52D54-2550-40CC-B4F2-E929121ED786}" mergeInterval="0" personalView="1" xWindow="540" yWindow="65" windowWidth="1440" windowHeight="759" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Ben Lee - 個人檢視畫面" guid="{C58F9881-D4DB-415A-8008-0AEBA40396F0}" mergeInterval="0" personalView="1" xWindow="88" yWindow="96" windowWidth="1780" windowHeight="941" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Cathy - 個人檢視畫面" guid="{717898C4-0574-484D-BD9C-6467A0CE5693}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="sylvie - 個人檢視畫面" guid="{63AF4A45-AD5B-4095-98AF-B9B7D76E853B}" mergeInterval="0" personalView="1" xWindow="70" yWindow="44" windowWidth="1792" windowHeight="939" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="alin - 個人檢視畫面" guid="{B7BC9F30-2585-4C16-9D81-4C9A56CF313D}" mergeInterval="0" personalView="1" xWindow="1943" yWindow="30" windowWidth="1612" windowHeight="984" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="franklee - 個人檢視畫面" guid="{0CCA00F3-751C-4787-8DCD-18810A223736}" mergeInterval="0" personalView="1" xWindow="2027" yWindow="82" windowWidth="1440" windowHeight="845" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Luke - 個人檢視畫面" guid="{D57EADF0-8313-4455-A499-88E2416AEB41}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Vicky - 個人檢視畫面" guid="{C85B642B-1BC6-4F60-ABA8-BB4902356EC7}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="barry - 個人檢視畫面" guid="{2798399B-15CB-4F8F-8B08-AAC3906FCE90}" mergeInterval="0" personalView="1" xWindow="1943" yWindow="140" windowWidth="1609" windowHeight="789" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Jay - 個人檢視畫面" guid="{BDE8CC60-A560-4175-ABA0-C6578D19736D}" mergeInterval="0" personalView="1" xWindow="299" yWindow="57" windowWidth="1440" windowHeight="821" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Rong - 個人檢視畫面" guid="{C52840BD-44C5-4DB3-87C8-6204EED81660}" mergeInterval="0" personalView="1" xWindow="2165" yWindow="12" windowWidth="1615" windowHeight="975" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="tim - 個人檢視畫面" guid="{65097A9F-84FB-4420-B9E1-55F003484CC9}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Amy - 個人檢視畫面" guid="{BE04F48D-7FB0-4A6B-8DA9-FD6977C1D755}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1874" windowHeight="1096" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Jan - 個人檢視畫面" guid="{C92EEC5E-992F-437E-ABC8-50A8EC09C45C}" mergeInterval="0" personalView="1" xWindow="101" yWindow="101" windowWidth="1698" windowHeight="929" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Ann - 個人檢視畫面" guid="{D181E684-8712-49C7-B0A7-7F095881A99A}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Roman - 個人檢視畫面" guid="{FCA4128F-7A64-4F78-A13C-88139C1F89EE}" mergeInterval="0" personalView="1" xWindow="2253" yWindow="96" windowWidth="1394" windowHeight="880" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="jeff - 個人檢視畫面" guid="{CCFABD62-875D-438A-AA81-F7901DFDF8D8}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Eric - 個人檢視畫面" guid="{6784737C-99C9-4A04-B57C-5D72318D91E8}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Samuel - 個人檢視畫面" guid="{AE954446-C682-4BA8-B992-13BC3C31A1A7}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Ming - 個人檢視畫面" guid="{EE49E775-74F1-4239-8BA7-B9013CF0869F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="abbie - 個人檢視畫面" guid="{0E00A347-0498-4A2B-AD80-BE12A213215B}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1874" windowHeight="1096" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="William - 個人檢視畫面" guid="{61077508-4D9D-4B00-AD48-DEF28B896630}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Weishih - 個人檢視畫面" guid="{4AC08E39-5641-4AA0-B7F4-0628373ED026}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Kai - 個人檢視畫面" guid="{BAAC823D-92DF-455D-8BAE-401D54AE0186}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Nancy - 個人檢視畫面" guid="{86F2BB6D-A835-405D-87BD-120D92ECC7FB}" mergeInterval="0" personalView="1" xWindow="363" yWindow="173" windowWidth="1515" windowHeight="795" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Mika - 個人檢視畫面" guid="{963ED05F-7C95-4FED-8B78-678C1C4B3B46}" mergeInterval="0" personalView="1" xWindow="1955" yWindow="411" windowWidth="1522" windowHeight="986" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="mars - 個人檢視畫面" guid="{39F1A034-65C6-4A53-BAC3-14F2537A4CDD}" mergeInterval="0" personalView="1" xWindow="254" yWindow="160" windowWidth="1440" windowHeight="759" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="George - 個人檢視畫面" guid="{AF17EE2E-1343-4F6F-8E18-F6DC3DA645FA}" mergeInterval="0" personalView="1" xWindow="283" yWindow="37" windowWidth="1749" windowHeight="759" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="mars - 個人檢視畫面" guid="{39F1A034-65C6-4A53-BAC3-14F2537A4CDD}" mergeInterval="0" personalView="1" xWindow="254" yWindow="160" windowWidth="1440" windowHeight="759" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Mika - 個人檢視畫面" guid="{963ED05F-7C95-4FED-8B78-678C1C4B3B46}" mergeInterval="0" personalView="1" xWindow="1955" yWindow="411" windowWidth="1522" windowHeight="986" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Nancy - 個人檢視畫面" guid="{86F2BB6D-A835-405D-87BD-120D92ECC7FB}" mergeInterval="0" personalView="1" xWindow="363" yWindow="173" windowWidth="1515" windowHeight="795" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Kai - 個人檢視畫面" guid="{BAAC823D-92DF-455D-8BAE-401D54AE0186}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Weishih - 個人檢視畫面" guid="{4AC08E39-5641-4AA0-B7F4-0628373ED026}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="William - 個人檢視畫面" guid="{61077508-4D9D-4B00-AD48-DEF28B896630}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="abbie - 個人檢視畫面" guid="{0E00A347-0498-4A2B-AD80-BE12A213215B}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1874" windowHeight="1096" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Ming - 個人檢視畫面" guid="{EE49E775-74F1-4239-8BA7-B9013CF0869F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Samuel - 個人檢視畫面" guid="{AE954446-C682-4BA8-B992-13BC3C31A1A7}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Eric - 個人檢視畫面" guid="{6784737C-99C9-4A04-B57C-5D72318D91E8}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="jeff - 個人檢視畫面" guid="{CCFABD62-875D-438A-AA81-F7901DFDF8D8}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Roman - 個人檢視畫面" guid="{FCA4128F-7A64-4F78-A13C-88139C1F89EE}" mergeInterval="0" personalView="1" xWindow="2253" yWindow="96" windowWidth="1394" windowHeight="880" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Ann - 個人檢視畫面" guid="{D181E684-8712-49C7-B0A7-7F095881A99A}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Jan - 個人檢視畫面" guid="{C92EEC5E-992F-437E-ABC8-50A8EC09C45C}" mergeInterval="0" personalView="1" xWindow="101" yWindow="101" windowWidth="1698" windowHeight="929" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Amy - 個人檢視畫面" guid="{BE04F48D-7FB0-4A6B-8DA9-FD6977C1D755}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1874" windowHeight="1096" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="tim - 個人檢視畫面" guid="{65097A9F-84FB-4420-B9E1-55F003484CC9}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Rong - 個人檢視畫面" guid="{C52840BD-44C5-4DB3-87C8-6204EED81660}" mergeInterval="0" personalView="1" xWindow="2165" yWindow="12" windowWidth="1615" windowHeight="975" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Jay - 個人檢視畫面" guid="{BDE8CC60-A560-4175-ABA0-C6578D19736D}" mergeInterval="0" personalView="1" xWindow="299" yWindow="57" windowWidth="1440" windowHeight="821" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="barry - 個人檢視畫面" guid="{2798399B-15CB-4F8F-8B08-AAC3906FCE90}" mergeInterval="0" personalView="1" xWindow="1943" yWindow="140" windowWidth="1609" windowHeight="789" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Vicky - 個人檢視畫面" guid="{C85B642B-1BC6-4F60-ABA8-BB4902356EC7}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Luke - 個人檢視畫面" guid="{D57EADF0-8313-4455-A499-88E2416AEB41}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="franklee - 個人檢視畫面" guid="{0CCA00F3-751C-4787-8DCD-18810A223736}" mergeInterval="0" personalView="1" xWindow="2027" yWindow="82" windowWidth="1440" windowHeight="845" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="alin - 個人檢視畫面" guid="{B7BC9F30-2585-4C16-9D81-4C9A56CF313D}" mergeInterval="0" personalView="1" xWindow="1943" yWindow="30" windowWidth="1612" windowHeight="984" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="sylvie - 個人檢視畫面" guid="{63AF4A45-AD5B-4095-98AF-B9B7D76E853B}" mergeInterval="0" personalView="1" xWindow="70" yWindow="44" windowWidth="1792" windowHeight="939" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Cathy - 個人檢視畫面" guid="{717898C4-0574-484D-BD9C-6467A0CE5693}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Ben Lee - 個人檢視畫面" guid="{C58F9881-D4DB-415A-8008-0AEBA40396F0}" mergeInterval="0" personalView="1" xWindow="88" yWindow="96" windowWidth="1780" windowHeight="941" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Jake - 個人檢視畫面" guid="{1DF52D54-2550-40CC-B4F2-E929121ED786}" mergeInterval="0" personalView="1" xWindow="540" yWindow="65" windowWidth="1440" windowHeight="759" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="vicwu - 個人檢視畫面" guid="{8817F74E-6F61-4E32-8724-D0D706F320DB}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
   <si>
     <t>FLC</t>
   </si>
@@ -1124,19 +1124,27 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>GT_Genesis For RGS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>GT_Genesis For Rad+</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>GT_Radi8 For RGS</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>GT_Radi8 For Rad+</t>
+    <t>GT_Genesis Part I</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>GT_Radi8 Part I</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>GT_Genesis Part II</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>GT_Radi8 Part II</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>GT_Genesis Part III</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>GT_Radi8 Part III</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1171,7 +1179,7 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1262,6 +1270,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1292,7 +1306,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1363,6 +1377,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1713,11 +1730,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -1729,10 +1746,11 @@
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.33203125" customWidth="1"/>
     <col min="7" max="7" width="17.33203125" customWidth="1"/>
-    <col min="8" max="1005" width="8.6640625" customWidth="1"/>
+    <col min="8" max="8" width="19.5" customWidth="1"/>
+    <col min="9" max="1005" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" s="21" t="s">
         <v>101</v>
       </c>
@@ -1743,16 +1761,22 @@
         <v>102</v>
       </c>
       <c r="D1" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="23" t="s">
         <v>104</v>
-      </c>
-      <c r="E1" s="23" t="s">
-        <v>103</v>
       </c>
       <c r="F1" s="23" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" s="2" customFormat="1">
+      <c r="G1" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1">
       <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
@@ -1775,8 +1799,16 @@
         <f>CONCATENATE(B2,"_gt_gns_02")</f>
         <v>A002_gt_gns_02</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" s="2" customFormat="1">
+      <c r="G2" s="2" t="str">
+        <f>CONCATENATE(A2, "_gt_gns_03")</f>
+        <v>XH_gt_gns_03</v>
+      </c>
+      <c r="H2" s="2" t="str">
+        <f>CONCATENATE(B2, "_gt_gns_03")</f>
+        <v>A002_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="2" customFormat="1">
       <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
@@ -1799,8 +1831,16 @@
         <f t="shared" ref="F3:F51" si="3">CONCATENATE(B3,"_gt_gns_02")</f>
         <v>A003_gt_gns_02</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" s="2" customFormat="1">
+      <c r="G3" s="2" t="str">
+        <f t="shared" ref="G3:G51" si="4">CONCATENATE(A3, "_gt_gns_03")</f>
+        <v>XAM_gt_gns_03</v>
+      </c>
+      <c r="H3" s="2" t="str">
+        <f t="shared" ref="H3:H51" si="5">CONCATENATE(B3, "_gt_gns_03")</f>
+        <v>A003_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="2" customFormat="1">
       <c r="A4" s="11" t="s">
         <v>3</v>
       </c>
@@ -1823,8 +1863,16 @@
         <f t="shared" si="3"/>
         <v>A004_gt_gns_02</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" s="2" customFormat="1">
+      <c r="G4" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>BLM_gt_gns_03</v>
+      </c>
+      <c r="H4" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A004_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="2" customFormat="1">
       <c r="A5" s="10" t="s">
         <v>10</v>
       </c>
@@ -1847,8 +1895,16 @@
         <f t="shared" si="3"/>
         <v>A005_gt_gns_02</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" s="2" customFormat="1">
+      <c r="G5" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>FHC_gt_gns_03</v>
+      </c>
+      <c r="H5" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A005_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="2" customFormat="1">
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
@@ -1871,8 +1927,16 @@
         <f t="shared" si="3"/>
         <v>A006_gt_gns_02</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" s="2" customFormat="1">
+      <c r="G6" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>KS_gt_gns_03</v>
+      </c>
+      <c r="H6" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A006_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="2" customFormat="1">
       <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
@@ -1895,8 +1959,16 @@
         <f t="shared" si="3"/>
         <v>A007_gt_gns_02</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" s="2" customFormat="1">
+      <c r="G7" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>JS_gt_gns_03</v>
+      </c>
+      <c r="H7" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A007_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="2" customFormat="1">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -1919,8 +1991,16 @@
         <f t="shared" si="3"/>
         <v>A009_gt_gns_02</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" s="2" customFormat="1">
+      <c r="G8" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>SJG_gt_gns_03</v>
+      </c>
+      <c r="H8" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A009_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="2" customFormat="1">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
@@ -1943,8 +2023,16 @@
         <f t="shared" si="3"/>
         <v>A011_gt_gns_02</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" s="2" customFormat="1">
+      <c r="G9" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>NXJ_gt_gns_03</v>
+      </c>
+      <c r="H9" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A011_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="2" customFormat="1">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -1967,8 +2055,16 @@
         <f t="shared" si="3"/>
         <v>A012_gt_gns_02</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" s="2" customFormat="1">
+      <c r="G10" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>HJC_gt_gns_03</v>
+      </c>
+      <c r="H10" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A012_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="2" customFormat="1">
       <c r="A11" s="13" t="s">
         <v>40</v>
       </c>
@@ -1991,8 +2087,16 @@
         <f t="shared" si="3"/>
         <v>A015_gt_gns_02</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" s="2" customFormat="1">
+      <c r="G11" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>YH_gt_gns_03</v>
+      </c>
+      <c r="H11" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A015_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="2" customFormat="1">
       <c r="A12" s="10" t="s">
         <v>14</v>
       </c>
@@ -2015,8 +2119,16 @@
         <f t="shared" si="3"/>
         <v>A017_gt_gns_02</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" s="2" customFormat="1">
+      <c r="G12" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>HJDC_gt_gns_03</v>
+      </c>
+      <c r="H12" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A017_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="2" customFormat="1">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
@@ -2039,8 +2151,16 @@
         <f t="shared" si="3"/>
         <v>A019_gt_gns_02</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" s="2" customFormat="1">
+      <c r="G13" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>BET_gt_gns_03</v>
+      </c>
+      <c r="H13" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A019_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="2" customFormat="1">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
@@ -2063,8 +2183,16 @@
         <f t="shared" si="3"/>
         <v>A020_gt_gns_02</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" s="2" customFormat="1">
+      <c r="G14" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>BAZR_gt_gns_03</v>
+      </c>
+      <c r="H14" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A020_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="2" customFormat="1">
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
@@ -2087,8 +2215,16 @@
         <f t="shared" si="3"/>
         <v>A022_gt_gns_02</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" s="2" customFormat="1">
+      <c r="G15" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>AMDC_gt_gns_03</v>
+      </c>
+      <c r="H15" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A022_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="2" customFormat="1">
       <c r="A16" s="5" t="s">
         <v>41</v>
       </c>
@@ -2111,8 +2247,16 @@
         <f t="shared" si="3"/>
         <v>A024_gt_gns_02</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" s="2" customFormat="1" ht="16">
+      <c r="G16" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>TYC_gt_gns_03</v>
+      </c>
+      <c r="H16" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A024_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="2" customFormat="1" ht="16">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -2135,8 +2279,16 @@
         <f t="shared" si="3"/>
         <v>A026_gt_gns_02</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" s="2" customFormat="1">
+      <c r="G17" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>BWIN_gt_gns_03</v>
+      </c>
+      <c r="H17" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A026_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="2" customFormat="1">
       <c r="A18" s="4" t="s">
         <v>6</v>
       </c>
@@ -2159,8 +2311,16 @@
         <f t="shared" si="3"/>
         <v>A027_gt_gns_02</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" s="2" customFormat="1">
+      <c r="G18" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>AMBC_gt_gns_03</v>
+      </c>
+      <c r="H18" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A027_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="2" customFormat="1">
       <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
@@ -2183,8 +2343,16 @@
         <f t="shared" si="3"/>
         <v>A029_gt_gns_02</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" s="2" customFormat="1">
+      <c r="G19" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>WLDB_gt_gns_03</v>
+      </c>
+      <c r="H19" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A029_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="2" customFormat="1">
       <c r="A20" s="4" t="s">
         <v>7</v>
       </c>
@@ -2207,8 +2375,16 @@
         <f t="shared" si="3"/>
         <v>A031_gt_gns_02</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" s="2" customFormat="1">
+      <c r="G20" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>AMZX_gt_gns_03</v>
+      </c>
+      <c r="H20" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A031_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="2" customFormat="1">
       <c r="A21" s="5" t="s">
         <v>46</v>
       </c>
@@ -2231,8 +2407,16 @@
         <f t="shared" si="3"/>
         <v>A032_gt_gns_02</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" s="2" customFormat="1">
+      <c r="G21" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>MS_gt_gns_03</v>
+      </c>
+      <c r="H21" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A032_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="2" customFormat="1">
       <c r="A22" s="3" t="s">
         <v>18</v>
       </c>
@@ -2255,8 +2439,16 @@
         <f t="shared" si="3"/>
         <v>A035_gt_gns_02</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" s="2" customFormat="1">
+      <c r="G22" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>BM_gt_gns_03</v>
+      </c>
+      <c r="H22" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A035_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="2" customFormat="1">
       <c r="A23" s="4" t="s">
         <v>27</v>
       </c>
@@ -2279,8 +2471,16 @@
         <f t="shared" si="3"/>
         <v>A036_gt_gns_02</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" s="2" customFormat="1">
+      <c r="G23" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>FLL_gt_gns_03</v>
+      </c>
+      <c r="H23" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A036_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="2" customFormat="1">
       <c r="A24" s="9" t="s">
         <v>28</v>
       </c>
@@ -2303,8 +2503,16 @@
         <f t="shared" si="3"/>
         <v>A041_gt_gns_02</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" s="2" customFormat="1">
+      <c r="G24" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>JBB_gt_gns_03</v>
+      </c>
+      <c r="H24" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A041_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="2" customFormat="1">
       <c r="A25" s="4" t="s">
         <v>8</v>
       </c>
@@ -2327,8 +2535,16 @@
         <f t="shared" si="3"/>
         <v>A043_gt_gns_02</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" s="2" customFormat="1">
+      <c r="G25" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>LB_gt_gns_03</v>
+      </c>
+      <c r="H25" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A043_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="2" customFormat="1">
       <c r="A26" s="4" t="s">
         <v>29</v>
       </c>
@@ -2351,8 +2567,16 @@
         <f t="shared" si="3"/>
         <v>A044_gt_gns_02</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" s="2" customFormat="1">
+      <c r="G26" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>AMGJ_gt_gns_03</v>
+      </c>
+      <c r="H26" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A044_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="2" customFormat="1">
       <c r="A27" s="5" t="s">
         <v>30</v>
       </c>
@@ -2375,8 +2599,16 @@
         <f t="shared" si="3"/>
         <v>A048_gt_gns_02</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" s="2" customFormat="1">
+      <c r="G27" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>WLYL_gt_gns_03</v>
+      </c>
+      <c r="H27" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A048_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="2" customFormat="1">
       <c r="A28" s="14" t="s">
         <v>31</v>
       </c>
@@ -2399,8 +2631,16 @@
         <f t="shared" si="3"/>
         <v>A049_gt_gns_02</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" s="2" customFormat="1" ht="16">
+      <c r="G28" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>KX8_gt_gns_03</v>
+      </c>
+      <c r="H28" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A049_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="2" customFormat="1" ht="16">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
@@ -2423,8 +2663,16 @@
         <f t="shared" si="3"/>
         <v>A051_gt_gns_02</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" s="2" customFormat="1">
+      <c r="G29" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>YF_gt_gns_03</v>
+      </c>
+      <c r="H29" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A051_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="2" customFormat="1">
       <c r="A30" s="4" t="s">
         <v>33</v>
       </c>
@@ -2447,8 +2695,16 @@
         <f t="shared" si="3"/>
         <v>A055_gt_gns_02</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" s="2" customFormat="1">
+      <c r="G30" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>MEDF_gt_gns_03</v>
+      </c>
+      <c r="H30" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A055_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="2" customFormat="1">
       <c r="A31" s="9" t="s">
         <v>9</v>
       </c>
@@ -2471,8 +2727,16 @@
         <f t="shared" si="3"/>
         <v>A056_gt_gns_02</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" s="2" customFormat="1">
+      <c r="G31" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>JW_gt_gns_03</v>
+      </c>
+      <c r="H31" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A056_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="2" customFormat="1">
       <c r="A32" s="9" t="s">
         <v>34</v>
       </c>
@@ -2495,8 +2759,16 @@
         <f t="shared" si="3"/>
         <v>A058_gt_gns_02</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" s="2" customFormat="1">
+      <c r="G32" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>SWJ_gt_gns_03</v>
+      </c>
+      <c r="H32" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A058_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="2" customFormat="1">
       <c r="A33" s="15" t="s">
         <v>0</v>
       </c>
@@ -2519,8 +2791,16 @@
         <f t="shared" si="3"/>
         <v>A059_gt_gns_02</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" s="2" customFormat="1">
+      <c r="G33" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>FLC_gt_gns_03</v>
+      </c>
+      <c r="H33" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A059_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="2" customFormat="1">
       <c r="A34" s="4" t="s">
         <v>35</v>
       </c>
@@ -2528,11 +2808,11 @@
         <v>86</v>
       </c>
       <c r="C34" s="2" t="str">
-        <f t="shared" ref="C34:C51" si="4">CONCATENATE(A34, "_gt_gns_01")</f>
+        <f t="shared" ref="C34:C51" si="6">CONCATENATE(A34, "_gt_gns_01")</f>
         <v>AMYH_gt_gns_01</v>
       </c>
       <c r="D34" s="2" t="str">
-        <f t="shared" ref="D34:D51" si="5">CONCATENATE(B34,"_gt_gns_01")</f>
+        <f t="shared" ref="D34:D51" si="7">CONCATENATE(B34,"_gt_gns_01")</f>
         <v>A064_gt_gns_01</v>
       </c>
       <c r="E34" s="2" t="str">
@@ -2543,8 +2823,16 @@
         <f t="shared" si="3"/>
         <v>A064_gt_gns_02</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" s="2" customFormat="1">
+      <c r="G34" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>AMYH_gt_gns_03</v>
+      </c>
+      <c r="H34" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A064_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="2" customFormat="1">
       <c r="A35" s="4" t="s">
         <v>36</v>
       </c>
@@ -2552,11 +2840,11 @@
         <v>97</v>
       </c>
       <c r="C35" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>GHH_gt_gns_01</v>
       </c>
       <c r="D35" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>A068_gt_gns_01</v>
       </c>
       <c r="E35" s="2" t="str">
@@ -2567,8 +2855,16 @@
         <f t="shared" si="3"/>
         <v>A068_gt_gns_02</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" s="2" customFormat="1">
+      <c r="G35" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>GHH_gt_gns_03</v>
+      </c>
+      <c r="H35" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A068_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="2" customFormat="1">
       <c r="A36" s="4" t="s">
         <v>37</v>
       </c>
@@ -2576,11 +2872,11 @@
         <v>87</v>
       </c>
       <c r="C36" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>WNSDC_gt_gns_01</v>
       </c>
       <c r="D36" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>A169_gt_gns_01</v>
       </c>
       <c r="E36" s="2" t="str">
@@ -2591,8 +2887,16 @@
         <f t="shared" si="3"/>
         <v>A169_gt_gns_02</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" s="2" customFormat="1">
+      <c r="G36" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>WNSDC_gt_gns_03</v>
+      </c>
+      <c r="H36" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A169_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="2" customFormat="1">
       <c r="A37" s="5" t="s">
         <v>38</v>
       </c>
@@ -2600,11 +2904,11 @@
         <v>88</v>
       </c>
       <c r="C37" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>XSDB_gt_gns_01</v>
       </c>
       <c r="D37" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>A170_gt_gns_01</v>
       </c>
       <c r="E37" s="2" t="str">
@@ -2615,8 +2919,16 @@
         <f t="shared" si="3"/>
         <v>A170_gt_gns_02</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" s="2" customFormat="1">
+      <c r="G37" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>XSDB_gt_gns_03</v>
+      </c>
+      <c r="H37" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A170_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="2" customFormat="1">
       <c r="A38" s="3" t="s">
         <v>21</v>
       </c>
@@ -2624,11 +2936,11 @@
         <v>77</v>
       </c>
       <c r="C38" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>BWWNS_gt_gns_01</v>
       </c>
       <c r="D38" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>A172_gt_gns_01</v>
       </c>
       <c r="E38" s="2" t="str">
@@ -2639,8 +2951,16 @@
         <f t="shared" si="3"/>
         <v>A172_gt_gns_02</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" s="2" customFormat="1">
+      <c r="G38" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>BWWNS_gt_gns_03</v>
+      </c>
+      <c r="H38" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A172_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="2" customFormat="1">
       <c r="A39" s="5" t="s">
         <v>24</v>
       </c>
@@ -2648,11 +2968,11 @@
         <v>79</v>
       </c>
       <c r="C39" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>BWBLR_gt_gns_01</v>
       </c>
       <c r="D39" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>A174_gt_gns_01</v>
       </c>
       <c r="E39" s="2" t="str">
@@ -2663,8 +2983,16 @@
         <f t="shared" si="3"/>
         <v>A174_gt_gns_02</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" s="2" customFormat="1">
+      <c r="G39" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>BWBLR_gt_gns_03</v>
+      </c>
+      <c r="H39" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A174_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="2" customFormat="1">
       <c r="A40" s="4" t="s">
         <v>22</v>
       </c>
@@ -2672,11 +3000,11 @@
         <v>98</v>
       </c>
       <c r="C40" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>BWBY_gt_gns_01</v>
       </c>
       <c r="D40" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>A175_gt_gns_01</v>
       </c>
       <c r="E40" s="2" t="str">
@@ -2687,8 +3015,16 @@
         <f t="shared" si="3"/>
         <v>A175_gt_gns_02</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" s="2" customFormat="1">
+      <c r="G40" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>BWBY_gt_gns_03</v>
+      </c>
+      <c r="H40" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A175_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" s="2" customFormat="1">
       <c r="A41" s="4" t="s">
         <v>25</v>
       </c>
@@ -2696,11 +3032,11 @@
         <v>80</v>
       </c>
       <c r="C41" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>BWYLG_gt_gns_01</v>
       </c>
       <c r="D41" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>A177_gt_gns_01</v>
       </c>
       <c r="E41" s="2" t="str">
@@ -2711,8 +3047,16 @@
         <f t="shared" si="3"/>
         <v>A177_gt_gns_02</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" s="2" customFormat="1">
+      <c r="G41" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>BWYLG_gt_gns_03</v>
+      </c>
+      <c r="H41" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A177_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" s="2" customFormat="1">
       <c r="A42" s="4" t="s">
         <v>23</v>
       </c>
@@ -2720,11 +3064,11 @@
         <v>99</v>
       </c>
       <c r="C42" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>BWBET_gt_gns_01</v>
       </c>
       <c r="D42" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>A179_gt_gns_01</v>
       </c>
       <c r="E42" s="2" t="str">
@@ -2735,8 +3079,16 @@
         <f t="shared" si="3"/>
         <v>A179_gt_gns_02</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" s="2" customFormat="1">
+      <c r="G42" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>BWBET_gt_gns_03</v>
+      </c>
+      <c r="H42" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A179_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" s="2" customFormat="1">
       <c r="A43" s="5" t="s">
         <v>42</v>
       </c>
@@ -2744,11 +3096,11 @@
         <v>96</v>
       </c>
       <c r="C43" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>PJDC_gt_gns_01</v>
       </c>
       <c r="D43" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>A180_gt_gns_01</v>
       </c>
       <c r="E43" s="2" t="str">
@@ -2759,8 +3111,16 @@
         <f t="shared" si="3"/>
         <v>A180_gt_gns_02</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" s="2" customFormat="1">
+      <c r="G43" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>PJDC_gt_gns_03</v>
+      </c>
+      <c r="H43" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A180_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" s="2" customFormat="1">
       <c r="A44" s="5" t="s">
         <v>47</v>
       </c>
@@ -2768,11 +3128,11 @@
         <v>78</v>
       </c>
       <c r="C44" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>YLAM_gt_gns_01</v>
       </c>
       <c r="D44" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>A186_gt_gns_01</v>
       </c>
       <c r="E44" s="2" t="str">
@@ -2783,8 +3143,16 @@
         <f t="shared" si="3"/>
         <v>A186_gt_gns_02</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" s="2" customFormat="1">
+      <c r="G44" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>YLAM_gt_gns_03</v>
+      </c>
+      <c r="H44" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A186_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" s="2" customFormat="1">
       <c r="A45" s="16" t="s">
         <v>48</v>
       </c>
@@ -2792,11 +3160,11 @@
         <v>95</v>
       </c>
       <c r="C45" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>DCMGM_gt_gns_01</v>
       </c>
       <c r="D45" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>A187_gt_gns_01</v>
       </c>
       <c r="E45" s="2" t="str">
@@ -2807,8 +3175,16 @@
         <f t="shared" si="3"/>
         <v>A187_gt_gns_02</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" s="2" customFormat="1">
+      <c r="G45" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>DCMGM_gt_gns_03</v>
+      </c>
+      <c r="H45" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A187_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" s="2" customFormat="1">
       <c r="A46" s="5" t="s">
         <v>43</v>
       </c>
@@ -2816,11 +3192,11 @@
         <v>94</v>
       </c>
       <c r="C46" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>PJYL_gt_gns_01</v>
       </c>
       <c r="D46" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>A191_gt_gns_01</v>
       </c>
       <c r="E46" s="2" t="str">
@@ -2831,8 +3207,16 @@
         <f t="shared" si="3"/>
         <v>A191_gt_gns_02</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" s="2" customFormat="1">
+      <c r="G46" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>PJYL_gt_gns_03</v>
+      </c>
+      <c r="H46" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A191_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="2" customFormat="1">
       <c r="A47" s="3" t="s">
         <v>26</v>
       </c>
@@ -2840,11 +3224,11 @@
         <v>81</v>
       </c>
       <c r="C47" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>BWYL_gt_gns_01</v>
       </c>
       <c r="D47" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>A193_gt_gns_01</v>
       </c>
       <c r="E47" s="2" t="str">
@@ -2855,8 +3239,16 @@
         <f t="shared" si="3"/>
         <v>A193_gt_gns_02</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" s="2" customFormat="1">
+      <c r="G47" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>BWYL_gt_gns_03</v>
+      </c>
+      <c r="H47" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A193_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" s="2" customFormat="1">
       <c r="A48" s="17" t="s">
         <v>39</v>
       </c>
@@ -2864,11 +3256,11 @@
         <v>93</v>
       </c>
       <c r="C48" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>YLHG_gt_gns_01</v>
       </c>
       <c r="D48" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>A200_gt_gns_01</v>
       </c>
       <c r="E48" s="2" t="str">
@@ -2879,8 +3271,16 @@
         <f t="shared" si="3"/>
         <v>A200_gt_gns_02</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" s="6" customFormat="1">
+      <c r="G48" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>YLHG_gt_gns_03</v>
+      </c>
+      <c r="H48" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A200_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" s="6" customFormat="1">
       <c r="A49" s="18" t="s">
         <v>44</v>
       </c>
@@ -2888,11 +3288,11 @@
         <v>52</v>
       </c>
       <c r="C49" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>AMBLR_gt_gns_01</v>
       </c>
       <c r="D49" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>A203_gt_gns_01</v>
       </c>
       <c r="E49" s="2" t="str">
@@ -2903,8 +3303,16 @@
         <f t="shared" si="3"/>
         <v>A203_gt_gns_02</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" s="6" customFormat="1">
+      <c r="G49" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>AMBLR_gt_gns_03</v>
+      </c>
+      <c r="H49" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A203_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" s="6" customFormat="1">
       <c r="A50" s="19" t="s">
         <v>45</v>
       </c>
@@ -2912,11 +3320,11 @@
         <v>92</v>
       </c>
       <c r="C50" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>WYNN_gt_gns_01</v>
       </c>
       <c r="D50" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>A205_gt_gns_01</v>
       </c>
       <c r="E50" s="2" t="str">
@@ -2927,8 +3335,16 @@
         <f t="shared" si="3"/>
         <v>A205_gt_gns_02</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" s="2" customFormat="1">
+      <c r="G50" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>WYNN_gt_gns_03</v>
+      </c>
+      <c r="H50" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A205_gt_gns_03</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" s="2" customFormat="1">
       <c r="A51" s="19" t="s">
         <v>49</v>
       </c>
@@ -2936,11 +3352,11 @@
         <v>91</v>
       </c>
       <c r="C51" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>HGOL_gt_gns_01</v>
       </c>
       <c r="D51" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>A208_gt_gns_01</v>
       </c>
       <c r="E51" s="2" t="str">
@@ -2950,6 +3366,14 @@
       <c r="F51" s="2" t="str">
         <f t="shared" si="3"/>
         <v>A208_gt_gns_02</v>
+      </c>
+      <c r="G51" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>HGOL_gt_gns_03</v>
+      </c>
+      <c r="H51" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>A208_gt_gns_03</v>
       </c>
     </row>
   </sheetData>
@@ -2957,131 +3381,53 @@
     <sortCondition ref="B1"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{AF17EE2E-1343-4F6F-8E18-F6DC3DA645FA}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+    <customSheetView guid="{8817F74E-6F61-4E32-8724-D0D706F320DB}">
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
       <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{39F1A034-65C6-4A53-BAC3-14F2537A4CDD}">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+    <customSheetView guid="{1DF52D54-2550-40CC-B4F2-E929121ED786}">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
       <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{963ED05F-7C95-4FED-8B78-678C1C4B3B46}">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C66" sqref="C66"/>
+    <customSheetView guid="{C58F9881-D4DB-415A-8008-0AEBA40396F0}">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
+      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
+      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+    </customSheetView>
+    <customSheetView guid="{717898C4-0574-484D-BD9C-6467A0CE5693}">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
+      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+    </customSheetView>
+    <customSheetView guid="{63AF4A45-AD5B-4095-98AF-B9B7D76E853B}">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C51" sqref="C51:D51"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
       <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{86F2BB6D-A835-405D-87BD-120D92ECC7FB}">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
+    <customSheetView guid="{B7BC9F30-2585-4C16-9D81-4C9A56CF313D}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
       <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{BAAC823D-92DF-455D-8BAE-401D54AE0186}">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
+    <customSheetView guid="{0CCA00F3-751C-4787-8DCD-18810A223736}">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
       <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
     </customSheetView>
-    <customSheetView guid="{4AC08E39-5641-4AA0-B7F4-0628373ED026}">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
-      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
-      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-    </customSheetView>
-    <customSheetView guid="{61077508-4D9D-4B00-AD48-DEF28B896630}">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
+    <customSheetView guid="{D57EADF0-8313-4455-A499-88E2416AEB41}" filter="1" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
       <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
-    </customSheetView>
-    <customSheetView guid="{0E00A347-0498-4A2B-AD80-BE12A213215B}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
-      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
-      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
-    </customSheetView>
-    <customSheetView guid="{EE49E775-74F1-4239-8BA7-B9013CF0869F}">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
-      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
-      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-    </customSheetView>
-    <customSheetView guid="{AE954446-C682-4BA8-B992-13BC3C31A1A7}">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E54" sqref="E54"/>
-      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
-      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
-    </customSheetView>
-    <customSheetView guid="{6784737C-99C9-4A04-B57C-5D72318D91E8}">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E64" sqref="E64"/>
-      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
-      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-    </customSheetView>
-    <customSheetView guid="{CCFABD62-875D-438A-AA81-F7901DFDF8D8}">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C65" sqref="C65"/>
-      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
-      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-    </customSheetView>
-    <customSheetView guid="{FCA4128F-7A64-4F78-A13C-88139C1F89EE}">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
-      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
-      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
-    </customSheetView>
-    <customSheetView guid="{D181E684-8712-49C7-B0A7-7F095881A99A}">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
-      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
-      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
-    </customSheetView>
-    <customSheetView guid="{C92EEC5E-992F-437E-ABC8-50A8EC09C45C}">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C75" sqref="C75"/>
-      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
-      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId10"/>
-    </customSheetView>
-    <customSheetView guid="{BE04F48D-7FB0-4A6B-8DA9-FD6977C1D755}">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
-      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
-      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>
-    </customSheetView>
-    <customSheetView guid="{65097A9F-84FB-4420-B9E1-55F003484CC9}">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
-      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
-      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>
-    </customSheetView>
-    <customSheetView guid="{C52840BD-44C5-4DB3-87C8-6204EED81660}">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C62" sqref="C62"/>
-      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
-      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId13"/>
-    </customSheetView>
-    <customSheetView guid="{BDE8CC60-A560-4175-ABA0-C6578D19736D}">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
-      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
-      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-    </customSheetView>
-    <customSheetView guid="{2798399B-15CB-4F8F-8B08-AAC3906FCE90}">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
-      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
-      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId14"/>
-    </customSheetView>
-    <customSheetView guid="{C85B642B-1BC6-4F60-ABA8-BB4902356EC7}" filter="1" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
-      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
-      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId15"/>
       <autoFilter ref="A1:G91" xr:uid="{00000000-0000-0000-0000-000000000000}">
         <filterColumn colId="1">
           <customFilters>
@@ -3090,11 +3436,11 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{D57EADF0-8313-4455-A499-88E2416AEB41}" filter="1" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+    <customSheetView guid="{C85B642B-1BC6-4F60-ABA8-BB4902356EC7}" filter="1" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
-      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId16"/>
+      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
       <autoFilter ref="A1:G91" xr:uid="{00000000-0000-0000-0000-000000000000}">
         <filterColumn colId="1">
           <customFilters>
@@ -3103,45 +3449,123 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{0CCA00F3-751C-4787-8DCD-18810A223736}">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
+    <customSheetView guid="{2798399B-15CB-4F8F-8B08-AAC3906FCE90}">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
+      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
+      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
+    </customSheetView>
+    <customSheetView guid="{BDE8CC60-A560-4175-ABA0-C6578D19736D}">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
       <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
     </customSheetView>
-    <customSheetView guid="{B7BC9F30-2585-4C16-9D81-4C9A56CF313D}">
+    <customSheetView guid="{C52840BD-44C5-4DB3-87C8-6204EED81660}">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C62" sqref="C62"/>
+      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
+      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
+    </customSheetView>
+    <customSheetView guid="{65097A9F-84FB-4420-B9E1-55F003484CC9}">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
+      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
+    </customSheetView>
+    <customSheetView guid="{BE04F48D-7FB0-4A6B-8DA9-FD6977C1D755}">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
+      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
+      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId10"/>
+    </customSheetView>
+    <customSheetView guid="{C92EEC5E-992F-437E-ABC8-50A8EC09C45C}">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C75" sqref="C75"/>
+      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
+      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>
+    </customSheetView>
+    <customSheetView guid="{D181E684-8712-49C7-B0A7-7F095881A99A}">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
+      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
+      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>
+    </customSheetView>
+    <customSheetView guid="{FCA4128F-7A64-4F78-A13C-88139C1F89EE}">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
+      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
+      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId13"/>
+    </customSheetView>
+    <customSheetView guid="{CCFABD62-875D-438A-AA81-F7901DFDF8D8}">
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C65" sqref="C65"/>
+      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
+      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+    </customSheetView>
+    <customSheetView guid="{6784737C-99C9-4A04-B57C-5D72318D91E8}">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E64" sqref="E64"/>
+      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
+      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+    </customSheetView>
+    <customSheetView guid="{AE954446-C682-4BA8-B992-13BC3C31A1A7}">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E54" sqref="E54"/>
+      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
+      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId14"/>
+    </customSheetView>
+    <customSheetView guid="{EE49E775-74F1-4239-8BA7-B9013CF0869F}">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
+      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
+      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+    </customSheetView>
+    <customSheetView guid="{0E00A347-0498-4A2B-AD80-BE12A213215B}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
+      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId15"/>
+    </customSheetView>
+    <customSheetView guid="{61077508-4D9D-4B00-AD48-DEF28B896630}">
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
+      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
+      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId16"/>
+    </customSheetView>
+    <customSheetView guid="{4AC08E39-5641-4AA0-B7F4-0628373ED026}">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
+      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+    </customSheetView>
+    <customSheetView guid="{BAAC823D-92DF-455D-8BAE-401D54AE0186}">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
+      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
+      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+    </customSheetView>
+    <customSheetView guid="{86F2BB6D-A835-405D-87BD-120D92ECC7FB}">
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
       <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId17"/>
     </customSheetView>
-    <customSheetView guid="{63AF4A45-AD5B-4095-98AF-B9B7D76E853B}">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C51" sqref="C51:D51"/>
+    <customSheetView guid="{963ED05F-7C95-4FED-8B78-678C1C4B3B46}">
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C66" sqref="C66"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
       <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId18"/>
     </customSheetView>
-    <customSheetView guid="{717898C4-0574-484D-BD9C-6467A0CE5693}">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
-      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
-      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-    </customSheetView>
-    <customSheetView guid="{C58F9881-D4DB-415A-8008-0AEBA40396F0}">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
-      <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
-      <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-    </customSheetView>
-    <customSheetView guid="{1DF52D54-2550-40CC-B4F2-E929121ED786}">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
+    <customSheetView guid="{39F1A034-65C6-4A53-BAC3-14F2537A4CDD}">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
       <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId19"/>
     </customSheetView>
-    <customSheetView guid="{8817F74E-6F61-4E32-8724-D0D706F320DB}">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
+    <customSheetView guid="{AF17EE2E-1343-4F6F-8E18-F6DC3DA645FA}">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
       <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
       <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId20"/>
     </customSheetView>

</xml_diff>